<commit_message>
adicionado os graficos de CET em funcao de numero de atomos
</commit_message>
<xml_diff>
--- a/num_atomos/crn128.xlsx
+++ b/num_atomos/crn128.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>CRN</t>
   </si>
@@ -116,21 +116,6 @@
   </si>
   <si>
     <t>crn_00024</t>
-  </si>
-  <si>
-    <t>crn_00025</t>
-  </si>
-  <si>
-    <t>crn_00026</t>
-  </si>
-  <si>
-    <t>crn_00027</t>
-  </si>
-  <si>
-    <t>crn_00028</t>
-  </si>
-  <si>
-    <t>crn_00029</t>
   </si>
 </sst>
 </file>
@@ -495,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -535,28 +520,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>884.843002</v>
+        <v>881.946489</v>
       </c>
       <c r="C2" s="2">
-        <v>271.945137</v>
+        <v>242.501927</v>
       </c>
       <c r="D2" s="2">
-        <v>0.073362</v>
+        <v>-0.140574</v>
       </c>
       <c r="E2" s="2">
-        <v>4.112274</v>
+        <v>1.86771</v>
       </c>
       <c r="F2" s="2">
-        <v>48.4375</v>
+        <v>54.6875</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2" s="2">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I2" s="2">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -564,28 +549,28 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>880.2731199999999</v>
+        <v>853.563088</v>
       </c>
       <c r="C3" s="2">
-        <v>242.032364</v>
+        <v>279.778026</v>
       </c>
       <c r="D3" s="2">
-        <v>0.223522</v>
+        <v>0.149223</v>
       </c>
       <c r="E3" s="2">
-        <v>4.462296</v>
+        <v>4.035843</v>
       </c>
       <c r="F3" s="2">
-        <v>48.4375</v>
+        <v>51.5625</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" s="2">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I3" s="2">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -593,28 +578,28 @@
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>909.154801</v>
+        <v>896.538497</v>
       </c>
       <c r="C4" s="2">
-        <v>230.853561</v>
+        <v>250.993333</v>
       </c>
       <c r="D4" s="2">
-        <v>0.764536</v>
+        <v>0.07372099999999999</v>
       </c>
       <c r="E4" s="2">
-        <v>6.125995</v>
+        <v>2.402375</v>
       </c>
       <c r="F4" s="2">
-        <v>48.4375</v>
+        <v>50</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="2">
+        <v>64</v>
+      </c>
+      <c r="I4" s="2">
         <v>62</v>
-      </c>
-      <c r="I4" s="2">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -622,28 +607,28 @@
         <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>881.072731</v>
+        <v>856.996006</v>
       </c>
       <c r="C5" s="2">
-        <v>234.826724</v>
+        <v>272.878538</v>
       </c>
       <c r="D5" s="2">
-        <v>0.044879</v>
+        <v>-0.087912</v>
       </c>
       <c r="E5" s="2">
-        <v>3.832187</v>
+        <v>3.494699</v>
       </c>
       <c r="F5" s="2">
-        <v>53.125</v>
+        <v>46.875</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
       </c>
       <c r="H5" s="2">
+        <v>60</v>
+      </c>
+      <c r="I5" s="2">
         <v>68</v>
-      </c>
-      <c r="I5" s="2">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -651,28 +636,28 @@
         <v>13</v>
       </c>
       <c r="B6" s="2">
-        <v>901.379146</v>
+        <v>858.837881</v>
       </c>
       <c r="C6" s="2">
-        <v>226.569736</v>
+        <v>230.82183</v>
       </c>
       <c r="D6" s="2">
-        <v>0.20704</v>
+        <v>-1.106368</v>
       </c>
       <c r="E6" s="2">
-        <v>3.78377</v>
+        <v>1.011564</v>
       </c>
       <c r="F6" s="2">
-        <v>45.3125</v>
+        <v>54.6875</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="I6" s="2">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -680,28 +665,28 @@
         <v>14</v>
       </c>
       <c r="B7" s="2">
-        <v>883.043088</v>
+        <v>913.830796</v>
       </c>
       <c r="C7" s="2">
-        <v>282.538835</v>
+        <v>230.691923</v>
       </c>
       <c r="D7" s="2">
-        <v>0.38336</v>
+        <v>0.04297</v>
       </c>
       <c r="E7" s="2">
-        <v>4.824149</v>
+        <v>4.832913</v>
       </c>
       <c r="F7" s="2">
         <v>48.4375</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2">
         <v>62</v>
       </c>
       <c r="I7" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -709,28 +694,28 @@
         <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>912.486714</v>
+        <v>861.931649</v>
       </c>
       <c r="C8" s="2">
-        <v>247.368769</v>
+        <v>241.958135</v>
       </c>
       <c r="D8" s="2">
-        <v>0.721716</v>
+        <v>0.173264</v>
       </c>
       <c r="E8" s="2">
-        <v>4.861198</v>
+        <v>5.955587</v>
       </c>
       <c r="F8" s="2">
-        <v>46.875</v>
+        <v>48.4375</v>
       </c>
       <c r="G8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I8" s="2">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -738,28 +723,28 @@
         <v>16</v>
       </c>
       <c r="B9" s="2">
-        <v>904.505726</v>
+        <v>856.319508</v>
       </c>
       <c r="C9" s="2">
-        <v>234.532404</v>
+        <v>248.282937</v>
       </c>
       <c r="D9" s="2">
-        <v>0.565748</v>
+        <v>0.08157300000000001</v>
       </c>
       <c r="E9" s="2">
-        <v>4.299237</v>
+        <v>3.69036</v>
       </c>
       <c r="F9" s="2">
-        <v>45.3125</v>
+        <v>53.125</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
       </c>
       <c r="H9" s="2">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="I9" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -767,28 +752,28 @@
         <v>17</v>
       </c>
       <c r="B10" s="2">
-        <v>920.035966</v>
+        <v>912.701227</v>
       </c>
       <c r="C10" s="2">
-        <v>221.916141</v>
+        <v>252.094699</v>
       </c>
       <c r="D10" s="2">
-        <v>-1.029606</v>
+        <v>0.033837</v>
       </c>
       <c r="E10" s="2">
-        <v>2.827604</v>
+        <v>2.180909</v>
       </c>
       <c r="F10" s="2">
-        <v>46.875</v>
+        <v>54.6875</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I10" s="2">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -796,28 +781,28 @@
         <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>896.761662</v>
+        <v>896.733764</v>
       </c>
       <c r="C11" s="2">
-        <v>238.759397</v>
+        <v>239.507313</v>
       </c>
       <c r="D11" s="2">
-        <v>0.06840300000000001</v>
+        <v>-0.182095</v>
       </c>
       <c r="E11" s="2">
-        <v>3.741863</v>
+        <v>2.141869</v>
       </c>
       <c r="F11" s="2">
-        <v>50</v>
+        <v>51.5625</v>
       </c>
       <c r="G11" s="2">
         <v>2</v>
       </c>
       <c r="H11" s="2">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I11" s="2">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -825,28 +810,28 @@
         <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>889.234745</v>
+        <v>902.100735</v>
       </c>
       <c r="C12" s="2">
-        <v>261.988056</v>
+        <v>245.857253</v>
       </c>
       <c r="D12" s="2">
-        <v>-0.380449</v>
+        <v>0.043037</v>
       </c>
       <c r="E12" s="2">
-        <v>1.696325</v>
+        <v>3.383029</v>
       </c>
       <c r="F12" s="2">
-        <v>46.875</v>
+        <v>54.6875</v>
       </c>
       <c r="G12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I12" s="2">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -854,28 +839,28 @@
         <v>20</v>
       </c>
       <c r="B13" s="2">
-        <v>931.080553</v>
+        <v>884.348984</v>
       </c>
       <c r="C13" s="2">
-        <v>246.306408</v>
+        <v>233.42138</v>
       </c>
       <c r="D13" s="2">
-        <v>0.605345</v>
+        <v>0.491044</v>
       </c>
       <c r="E13" s="2">
-        <v>3.240956</v>
+        <v>5.890886</v>
       </c>
       <c r="F13" s="2">
         <v>46.875</v>
       </c>
       <c r="G13" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" s="2">
         <v>60</v>
       </c>
       <c r="I13" s="2">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -883,16 +868,16 @@
         <v>21</v>
       </c>
       <c r="B14" s="2">
-        <v>940.77688</v>
+        <v>891.0269479999999</v>
       </c>
       <c r="C14" s="2">
-        <v>259.021261</v>
+        <v>269.382221</v>
       </c>
       <c r="D14" s="2">
-        <v>1.304644</v>
+        <v>-0.266904</v>
       </c>
       <c r="E14" s="2">
-        <v>9.343798</v>
+        <v>2.821687</v>
       </c>
       <c r="F14" s="2">
         <v>46.875</v>
@@ -912,28 +897,28 @@
         <v>22</v>
       </c>
       <c r="B15" s="2">
-        <v>916.361865</v>
+        <v>861.334028</v>
       </c>
       <c r="C15" s="2">
-        <v>249.821152</v>
+        <v>256.452531</v>
       </c>
       <c r="D15" s="2">
-        <v>0.371368</v>
+        <v>0.120206</v>
       </c>
       <c r="E15" s="2">
-        <v>5.771617</v>
+        <v>2.916221</v>
       </c>
       <c r="F15" s="2">
-        <v>45.3125</v>
+        <v>50</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="I15" s="2">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -941,28 +926,28 @@
         <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>896.788165</v>
+        <v>873.613148</v>
       </c>
       <c r="C16" s="2">
-        <v>239.456846</v>
+        <v>231.483972</v>
       </c>
       <c r="D16" s="2">
-        <v>-1.029416</v>
+        <v>0.269043</v>
       </c>
       <c r="E16" s="2">
-        <v>2.104438</v>
+        <v>5.332094</v>
       </c>
       <c r="F16" s="2">
-        <v>48.4375</v>
+        <v>54.6875</v>
       </c>
       <c r="G16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I16" s="2">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -970,28 +955,28 @@
         <v>24</v>
       </c>
       <c r="B17" s="2">
-        <v>881.527465</v>
+        <v>895.562584</v>
       </c>
       <c r="C17" s="2">
-        <v>230.67792</v>
+        <v>219.485318</v>
       </c>
       <c r="D17" s="2">
-        <v>0.125208</v>
+        <v>-1.399416</v>
       </c>
       <c r="E17" s="2">
-        <v>3.425094</v>
+        <v>1.298312</v>
       </c>
       <c r="F17" s="2">
-        <v>54.6875</v>
+        <v>50</v>
       </c>
       <c r="G17" s="2">
         <v>2</v>
       </c>
       <c r="H17" s="2">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I17" s="2">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -999,28 +984,28 @@
         <v>25</v>
       </c>
       <c r="B18" s="2">
-        <v>913.458218</v>
+        <v>866.6680249999999</v>
       </c>
       <c r="C18" s="2">
-        <v>238.412568</v>
+        <v>263.282676</v>
       </c>
       <c r="D18" s="2">
-        <v>-0.583194</v>
+        <v>1.151636</v>
       </c>
       <c r="E18" s="2">
-        <v>5.863631</v>
+        <v>5.725297</v>
       </c>
       <c r="F18" s="2">
-        <v>50</v>
+        <v>48.4375</v>
       </c>
       <c r="G18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="2">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I18" s="2">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1028,28 +1013,28 @@
         <v>26</v>
       </c>
       <c r="B19" s="2">
-        <v>902.332666</v>
+        <v>856.671243</v>
       </c>
       <c r="C19" s="2">
-        <v>247.598781</v>
+        <v>247.115408</v>
       </c>
       <c r="D19" s="2">
-        <v>0.452485</v>
+        <v>-0.533533</v>
       </c>
       <c r="E19" s="2">
-        <v>3.658795</v>
+        <v>1.937697</v>
       </c>
       <c r="F19" s="2">
-        <v>54.6875</v>
+        <v>53.125</v>
       </c>
       <c r="G19" s="2">
         <v>1</v>
       </c>
       <c r="H19" s="2">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I19" s="2">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1057,28 +1042,28 @@
         <v>27</v>
       </c>
       <c r="B20" s="2">
-        <v>888.213688</v>
+        <v>874.655362</v>
       </c>
       <c r="C20" s="2">
-        <v>283.308339</v>
+        <v>245.966022</v>
       </c>
       <c r="D20" s="2">
-        <v>0.039979</v>
+        <v>0.326655</v>
       </c>
       <c r="E20" s="2">
-        <v>5.043244</v>
+        <v>4.382966</v>
       </c>
       <c r="F20" s="2">
-        <v>54.6875</v>
+        <v>48.4375</v>
       </c>
       <c r="G20" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20" s="2">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I20" s="2">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1086,28 +1071,28 @@
         <v>28</v>
       </c>
       <c r="B21" s="2">
-        <v>888.170168</v>
+        <v>888.2242220000001</v>
       </c>
       <c r="C21" s="2">
-        <v>266.732914</v>
+        <v>245.693509</v>
       </c>
       <c r="D21" s="2">
-        <v>0.105147</v>
+        <v>0.188066</v>
       </c>
       <c r="E21" s="2">
-        <v>3.381397</v>
+        <v>3.193398</v>
       </c>
       <c r="F21" s="2">
-        <v>45.3125</v>
+        <v>51.5625</v>
       </c>
       <c r="G21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" s="2">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="I21" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1115,28 +1100,28 @@
         <v>29</v>
       </c>
       <c r="B22" s="2">
-        <v>858.98155</v>
+        <v>893.807727</v>
       </c>
       <c r="C22" s="2">
-        <v>274.596332</v>
+        <v>254.932305</v>
       </c>
       <c r="D22" s="2">
-        <v>1.166528</v>
+        <v>0.482877</v>
       </c>
       <c r="E22" s="2">
-        <v>9.720386</v>
+        <v>5.395766</v>
       </c>
       <c r="F22" s="2">
         <v>46.875</v>
       </c>
       <c r="G22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2">
         <v>60</v>
       </c>
       <c r="I22" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1144,28 +1129,28 @@
         <v>30</v>
       </c>
       <c r="B23" s="2">
-        <v>878.955274</v>
+        <v>843.694317</v>
       </c>
       <c r="C23" s="2">
-        <v>277.423116</v>
+        <v>252.224038</v>
       </c>
       <c r="D23" s="2">
-        <v>0.463572</v>
+        <v>0.142732</v>
       </c>
       <c r="E23" s="2">
-        <v>3.534349</v>
+        <v>7.942065</v>
       </c>
       <c r="F23" s="2">
-        <v>45.3125</v>
+        <v>48.4375</v>
       </c>
       <c r="G23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I23" s="2">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1173,28 +1158,28 @@
         <v>31</v>
       </c>
       <c r="B24" s="2">
-        <v>870.599787</v>
+        <v>886.506652</v>
       </c>
       <c r="C24" s="2">
-        <v>286.122453</v>
+        <v>272.621458</v>
       </c>
       <c r="D24" s="2">
-        <v>-0.174218</v>
+        <v>-0.449558</v>
       </c>
       <c r="E24" s="2">
-        <v>3.077616</v>
+        <v>1.864205</v>
       </c>
       <c r="F24" s="2">
-        <v>43.75</v>
+        <v>54.6875</v>
       </c>
       <c r="G24" s="2">
         <v>0</v>
       </c>
       <c r="H24" s="2">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="I24" s="2">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1202,28 +1187,28 @@
         <v>32</v>
       </c>
       <c r="B25" s="2">
-        <v>883.756517</v>
+        <v>898.185211</v>
       </c>
       <c r="C25" s="2">
-        <v>275.719967</v>
+        <v>257.13574</v>
       </c>
       <c r="D25" s="2">
-        <v>-0.490582</v>
+        <v>-0.46345</v>
       </c>
       <c r="E25" s="2">
-        <v>1.973684</v>
+        <v>4.197988</v>
       </c>
       <c r="F25" s="2">
-        <v>48.4375</v>
+        <v>51.5625</v>
       </c>
       <c r="G25" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25" s="2">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I25" s="2">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1231,173 +1216,28 @@
         <v>33</v>
       </c>
       <c r="B26" s="2">
-        <v>893.867855</v>
+        <v>869.643886</v>
       </c>
       <c r="C26" s="2">
-        <v>246.397751</v>
+        <v>262.298498</v>
       </c>
       <c r="D26" s="2">
-        <v>0.422662</v>
+        <v>-0.933485</v>
       </c>
       <c r="E26" s="2">
-        <v>3.359233</v>
+        <v>2.552094</v>
       </c>
       <c r="F26" s="2">
-        <v>50</v>
+        <v>45.3125</v>
       </c>
       <c r="G26" s="2">
         <v>0</v>
       </c>
       <c r="H26" s="2">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I26" s="2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="2">
-        <v>862.238987</v>
-      </c>
-      <c r="C27" s="2">
-        <v>277.164759</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.224834</v>
-      </c>
-      <c r="E27" s="2">
-        <v>5.055178</v>
-      </c>
-      <c r="F27" s="2">
-        <v>45.3125</v>
-      </c>
-      <c r="G27" s="2">
-        <v>1</v>
-      </c>
-      <c r="H27" s="2">
-        <v>58</v>
-      </c>
-      <c r="I27" s="2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="2">
-        <v>884.219083</v>
-      </c>
-      <c r="C28" s="2">
-        <v>248.273829</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.065063</v>
-      </c>
-      <c r="E28" s="2">
-        <v>3.720214</v>
-      </c>
-      <c r="F28" s="2">
-        <v>54.6875</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
         <v>70</v>
-      </c>
-      <c r="I28" s="2">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="2">
-        <v>888.351466</v>
-      </c>
-      <c r="C29" s="2">
-        <v>252.311161</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.259043</v>
-      </c>
-      <c r="E29" s="2">
-        <v>3.580078</v>
-      </c>
-      <c r="F29" s="2">
-        <v>45.3125</v>
-      </c>
-      <c r="G29" s="2">
-        <v>2</v>
-      </c>
-      <c r="H29" s="2">
-        <v>58</v>
-      </c>
-      <c r="I29" s="2">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="2">
-        <v>874.514615</v>
-      </c>
-      <c r="C30" s="2">
-        <v>238.339097</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.032151</v>
-      </c>
-      <c r="E30" s="2">
-        <v>2.741776</v>
-      </c>
-      <c r="F30" s="2">
-        <v>46.875</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>60</v>
-      </c>
-      <c r="I30" s="2">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="2">
-        <v>898.182139</v>
-      </c>
-      <c r="C31" s="2">
-        <v>283.848044</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.157372</v>
-      </c>
-      <c r="E31" s="2">
-        <v>2.871452</v>
-      </c>
-      <c r="F31" s="2">
-        <v>50</v>
-      </c>
-      <c r="G31" s="2">
-        <v>1</v>
-      </c>
-      <c r="H31" s="2">
-        <v>64</v>
-      </c>
-      <c r="I31" s="2">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CET em funcao do numero de atomos
</commit_message>
<xml_diff>
--- a/num_atomos/crn128.xlsx
+++ b/num_atomos/crn128.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>CRN</t>
   </si>
@@ -116,6 +116,21 @@
   </si>
   <si>
     <t>crn_00024</t>
+  </si>
+  <si>
+    <t>crn_00025</t>
+  </si>
+  <si>
+    <t>crn_00026</t>
+  </si>
+  <si>
+    <t>crn_00027</t>
+  </si>
+  <si>
+    <t>crn_00028</t>
+  </si>
+  <si>
+    <t>crn_00029</t>
   </si>
 </sst>
 </file>
@@ -480,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -520,28 +535,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>881.946489</v>
+        <v>871.0112360000001</v>
       </c>
       <c r="C2" s="2">
-        <v>242.501927</v>
+        <v>257.805191</v>
       </c>
       <c r="D2" s="2">
-        <v>-0.140574</v>
+        <v>1.107013</v>
       </c>
       <c r="E2" s="2">
-        <v>1.86771</v>
+        <v>7.83053</v>
       </c>
       <c r="F2" s="2">
-        <v>54.6875</v>
+        <v>50</v>
       </c>
       <c r="G2" s="2">
         <v>2</v>
       </c>
       <c r="H2" s="2">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I2" s="2">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -549,28 +564,28 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>853.563088</v>
+        <v>873.174569</v>
       </c>
       <c r="C3" s="2">
-        <v>279.778026</v>
+        <v>231.377293</v>
       </c>
       <c r="D3" s="2">
-        <v>0.149223</v>
+        <v>0.029002</v>
       </c>
       <c r="E3" s="2">
-        <v>4.035843</v>
+        <v>4.592623</v>
       </c>
       <c r="F3" s="2">
-        <v>51.5625</v>
+        <v>53.125</v>
       </c>
       <c r="G3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="2">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I3" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -578,28 +593,28 @@
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>896.538497</v>
+        <v>862.094684</v>
       </c>
       <c r="C4" s="2">
-        <v>250.993333</v>
+        <v>250.665492</v>
       </c>
       <c r="D4" s="2">
-        <v>0.07372099999999999</v>
+        <v>-2.369145</v>
       </c>
       <c r="E4" s="2">
-        <v>2.402375</v>
+        <v>0.680936</v>
       </c>
       <c r="F4" s="2">
-        <v>50</v>
+        <v>45.3125</v>
       </c>
       <c r="G4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" s="2">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I4" s="2">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -607,28 +622,28 @@
         <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>856.996006</v>
+        <v>867.26811</v>
       </c>
       <c r="C5" s="2">
-        <v>272.878538</v>
+        <v>220.789683</v>
       </c>
       <c r="D5" s="2">
-        <v>-0.087912</v>
+        <v>0.173808</v>
       </c>
       <c r="E5" s="2">
-        <v>3.494699</v>
+        <v>7.256983</v>
       </c>
       <c r="F5" s="2">
-        <v>46.875</v>
+        <v>54.6875</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H5" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I5" s="2">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -636,28 +651,28 @@
         <v>13</v>
       </c>
       <c r="B6" s="2">
-        <v>858.837881</v>
+        <v>842.596559</v>
       </c>
       <c r="C6" s="2">
-        <v>230.82183</v>
+        <v>234.21166</v>
       </c>
       <c r="D6" s="2">
-        <v>-1.106368</v>
+        <v>5.926872</v>
       </c>
       <c r="E6" s="2">
-        <v>1.011564</v>
+        <v>34.730584</v>
       </c>
       <c r="F6" s="2">
         <v>54.6875</v>
       </c>
       <c r="G6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2">
         <v>70</v>
       </c>
       <c r="I6" s="2">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -665,28 +680,28 @@
         <v>14</v>
       </c>
       <c r="B7" s="2">
-        <v>913.830796</v>
+        <v>904.960629</v>
       </c>
       <c r="C7" s="2">
-        <v>230.691923</v>
+        <v>254.428844</v>
       </c>
       <c r="D7" s="2">
-        <v>0.04297</v>
+        <v>2.863191</v>
       </c>
       <c r="E7" s="2">
-        <v>4.832913</v>
+        <v>15.61796</v>
       </c>
       <c r="F7" s="2">
-        <v>48.4375</v>
+        <v>50</v>
       </c>
       <c r="G7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I7" s="2">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -694,28 +709,28 @@
         <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>861.931649</v>
+        <v>844.846649</v>
       </c>
       <c r="C8" s="2">
-        <v>241.958135</v>
+        <v>269.202894</v>
       </c>
       <c r="D8" s="2">
-        <v>0.173264</v>
+        <v>0.099444</v>
       </c>
       <c r="E8" s="2">
-        <v>5.955587</v>
+        <v>4.735319</v>
       </c>
       <c r="F8" s="2">
-        <v>48.4375</v>
+        <v>51.5625</v>
       </c>
       <c r="G8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I8" s="2">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -723,28 +738,28 @@
         <v>16</v>
       </c>
       <c r="B9" s="2">
-        <v>856.319508</v>
+        <v>864.188796</v>
       </c>
       <c r="C9" s="2">
-        <v>248.282937</v>
+        <v>247.48918</v>
       </c>
       <c r="D9" s="2">
-        <v>0.08157300000000001</v>
+        <v>0.032859</v>
       </c>
       <c r="E9" s="2">
-        <v>3.69036</v>
+        <v>2.498639</v>
       </c>
       <c r="F9" s="2">
-        <v>53.125</v>
+        <v>45.3125</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H9" s="2">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="I9" s="2">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -752,28 +767,28 @@
         <v>17</v>
       </c>
       <c r="B10" s="2">
-        <v>912.701227</v>
+        <v>862.121858</v>
       </c>
       <c r="C10" s="2">
-        <v>252.094699</v>
+        <v>256.141665</v>
       </c>
       <c r="D10" s="2">
-        <v>0.033837</v>
+        <v>0.6160870000000001</v>
       </c>
       <c r="E10" s="2">
-        <v>2.180909</v>
+        <v>4.858</v>
       </c>
       <c r="F10" s="2">
-        <v>54.6875</v>
+        <v>50</v>
       </c>
       <c r="G10" s="2">
         <v>2</v>
       </c>
       <c r="H10" s="2">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I10" s="2">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -781,28 +796,28 @@
         <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>896.733764</v>
+        <v>856.076057</v>
       </c>
       <c r="C11" s="2">
-        <v>239.507313</v>
+        <v>241.177543</v>
       </c>
       <c r="D11" s="2">
-        <v>-0.182095</v>
+        <v>2.153683</v>
       </c>
       <c r="E11" s="2">
-        <v>2.141869</v>
+        <v>11.602145</v>
       </c>
       <c r="F11" s="2">
-        <v>51.5625</v>
+        <v>54.6875</v>
       </c>
       <c r="G11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="2">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I11" s="2">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -810,28 +825,28 @@
         <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>902.100735</v>
+        <v>853.887066</v>
       </c>
       <c r="C12" s="2">
-        <v>245.857253</v>
+        <v>283.605365</v>
       </c>
       <c r="D12" s="2">
-        <v>0.043037</v>
+        <v>0.310456</v>
       </c>
       <c r="E12" s="2">
-        <v>3.383029</v>
+        <v>5.5937</v>
       </c>
       <c r="F12" s="2">
-        <v>54.6875</v>
+        <v>46.875</v>
       </c>
       <c r="G12" s="2">
         <v>2</v>
       </c>
       <c r="H12" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I12" s="2">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -839,28 +854,28 @@
         <v>20</v>
       </c>
       <c r="B13" s="2">
-        <v>884.348984</v>
+        <v>873.448664</v>
       </c>
       <c r="C13" s="2">
-        <v>233.42138</v>
+        <v>267.758317</v>
       </c>
       <c r="D13" s="2">
-        <v>0.491044</v>
+        <v>-0.011156</v>
       </c>
       <c r="E13" s="2">
-        <v>5.890886</v>
+        <v>5.760397</v>
       </c>
       <c r="F13" s="2">
         <v>46.875</v>
       </c>
       <c r="G13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13" s="2">
         <v>60</v>
       </c>
       <c r="I13" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -868,28 +883,28 @@
         <v>21</v>
       </c>
       <c r="B14" s="2">
-        <v>891.0269479999999</v>
+        <v>877.59447</v>
       </c>
       <c r="C14" s="2">
-        <v>269.382221</v>
+        <v>256.374091</v>
       </c>
       <c r="D14" s="2">
-        <v>-0.266904</v>
+        <v>-0.478993</v>
       </c>
       <c r="E14" s="2">
-        <v>2.821687</v>
+        <v>2.114145</v>
       </c>
       <c r="F14" s="2">
-        <v>46.875</v>
+        <v>53.125</v>
       </c>
       <c r="G14" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H14" s="2">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="I14" s="2">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -897,28 +912,28 @@
         <v>22</v>
       </c>
       <c r="B15" s="2">
-        <v>861.334028</v>
+        <v>860.248153</v>
       </c>
       <c r="C15" s="2">
-        <v>256.452531</v>
+        <v>251.468366</v>
       </c>
       <c r="D15" s="2">
-        <v>0.120206</v>
+        <v>0.323785</v>
       </c>
       <c r="E15" s="2">
-        <v>2.916221</v>
+        <v>3.561581</v>
       </c>
       <c r="F15" s="2">
-        <v>50</v>
+        <v>54.6875</v>
       </c>
       <c r="G15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I15" s="2">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -926,28 +941,28 @@
         <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>873.613148</v>
+        <v>861.279713</v>
       </c>
       <c r="C16" s="2">
-        <v>231.483972</v>
+        <v>272.54073</v>
       </c>
       <c r="D16" s="2">
-        <v>0.269043</v>
+        <v>0.201327</v>
       </c>
       <c r="E16" s="2">
-        <v>5.332094</v>
+        <v>4.48071</v>
       </c>
       <c r="F16" s="2">
-        <v>54.6875</v>
+        <v>51.5625</v>
       </c>
       <c r="G16" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="2">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I16" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -955,28 +970,28 @@
         <v>24</v>
       </c>
       <c r="B17" s="2">
-        <v>895.562584</v>
+        <v>883.299083</v>
       </c>
       <c r="C17" s="2">
-        <v>219.485318</v>
+        <v>235.417525</v>
       </c>
       <c r="D17" s="2">
-        <v>-1.399416</v>
+        <v>2.339854</v>
       </c>
       <c r="E17" s="2">
-        <v>1.298312</v>
+        <v>30.465007</v>
       </c>
       <c r="F17" s="2">
         <v>50</v>
       </c>
       <c r="G17" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17" s="2">
         <v>64</v>
       </c>
       <c r="I17" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -984,28 +999,28 @@
         <v>25</v>
       </c>
       <c r="B18" s="2">
-        <v>866.6680249999999</v>
+        <v>856.319508</v>
       </c>
       <c r="C18" s="2">
-        <v>263.282676</v>
+        <v>278.482293</v>
       </c>
       <c r="D18" s="2">
-        <v>1.151636</v>
+        <v>-0.509336</v>
       </c>
       <c r="E18" s="2">
-        <v>5.725297</v>
+        <v>2.914026</v>
       </c>
       <c r="F18" s="2">
-        <v>48.4375</v>
+        <v>45.3125</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
       </c>
       <c r="H18" s="2">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I18" s="2">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1013,28 +1028,28 @@
         <v>26</v>
       </c>
       <c r="B19" s="2">
-        <v>856.671243</v>
+        <v>846.026864</v>
       </c>
       <c r="C19" s="2">
-        <v>247.115408</v>
+        <v>263.035889</v>
       </c>
       <c r="D19" s="2">
-        <v>-0.533533</v>
+        <v>0.065183</v>
       </c>
       <c r="E19" s="2">
-        <v>1.937697</v>
+        <v>5.93822</v>
       </c>
       <c r="F19" s="2">
-        <v>53.125</v>
+        <v>50</v>
       </c>
       <c r="G19" s="2">
         <v>1</v>
       </c>
       <c r="H19" s="2">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I19" s="2">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1042,28 +1057,28 @@
         <v>27</v>
       </c>
       <c r="B20" s="2">
-        <v>874.655362</v>
+        <v>881.367229</v>
       </c>
       <c r="C20" s="2">
-        <v>245.966022</v>
+        <v>213.648102</v>
       </c>
       <c r="D20" s="2">
-        <v>0.326655</v>
+        <v>-0.569958</v>
       </c>
       <c r="E20" s="2">
-        <v>4.382966</v>
+        <v>1.340945</v>
       </c>
       <c r="F20" s="2">
-        <v>48.4375</v>
+        <v>54.6875</v>
       </c>
       <c r="G20" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20" s="2">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I20" s="2">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1071,28 +1086,28 @@
         <v>28</v>
       </c>
       <c r="B21" s="2">
-        <v>888.2242220000001</v>
+        <v>892.472232</v>
       </c>
       <c r="C21" s="2">
-        <v>245.693509</v>
+        <v>247.529616</v>
       </c>
       <c r="D21" s="2">
-        <v>0.188066</v>
+        <v>-0.307756</v>
       </c>
       <c r="E21" s="2">
-        <v>3.193398</v>
+        <v>2.603753</v>
       </c>
       <c r="F21" s="2">
-        <v>51.5625</v>
+        <v>50</v>
       </c>
       <c r="G21" s="2">
         <v>2</v>
       </c>
       <c r="H21" s="2">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I21" s="2">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1100,28 +1115,28 @@
         <v>29</v>
       </c>
       <c r="B22" s="2">
-        <v>893.807727</v>
+        <v>864.4337839999999</v>
       </c>
       <c r="C22" s="2">
-        <v>254.932305</v>
+        <v>247.761817</v>
       </c>
       <c r="D22" s="2">
-        <v>0.482877</v>
+        <v>0.040677</v>
       </c>
       <c r="E22" s="2">
-        <v>5.395766</v>
+        <v>2.494565</v>
       </c>
       <c r="F22" s="2">
-        <v>46.875</v>
+        <v>51.5625</v>
       </c>
       <c r="G22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="2">
+        <v>66</v>
+      </c>
+      <c r="I22" s="2">
         <v>60</v>
-      </c>
-      <c r="I22" s="2">
-        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1129,28 +1144,28 @@
         <v>30</v>
       </c>
       <c r="B23" s="2">
-        <v>843.694317</v>
+        <v>877.1545589999999</v>
       </c>
       <c r="C23" s="2">
-        <v>252.224038</v>
+        <v>273.594081</v>
       </c>
       <c r="D23" s="2">
-        <v>0.142732</v>
+        <v>0.056319</v>
       </c>
       <c r="E23" s="2">
-        <v>7.942065</v>
+        <v>3.804761</v>
       </c>
       <c r="F23" s="2">
-        <v>48.4375</v>
+        <v>50</v>
       </c>
       <c r="G23" s="2">
         <v>1</v>
       </c>
       <c r="H23" s="2">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I23" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1158,28 +1173,28 @@
         <v>31</v>
       </c>
       <c r="B24" s="2">
-        <v>886.506652</v>
+        <v>869.315935</v>
       </c>
       <c r="C24" s="2">
-        <v>272.621458</v>
+        <v>242.165303</v>
       </c>
       <c r="D24" s="2">
-        <v>-0.449558</v>
+        <v>0.200015</v>
       </c>
       <c r="E24" s="2">
-        <v>1.864205</v>
+        <v>8.358812</v>
       </c>
       <c r="F24" s="2">
-        <v>54.6875</v>
+        <v>50</v>
       </c>
       <c r="G24" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H24" s="2">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I24" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1187,28 +1202,28 @@
         <v>32</v>
       </c>
       <c r="B25" s="2">
-        <v>898.185211</v>
+        <v>860.7095389999999</v>
       </c>
       <c r="C25" s="2">
-        <v>257.13574</v>
+        <v>277.149964</v>
       </c>
       <c r="D25" s="2">
-        <v>-0.46345</v>
+        <v>0.158575</v>
       </c>
       <c r="E25" s="2">
-        <v>4.197988</v>
+        <v>3.952814</v>
       </c>
       <c r="F25" s="2">
-        <v>51.5625</v>
+        <v>46.875</v>
       </c>
       <c r="G25" s="2">
         <v>2</v>
       </c>
       <c r="H25" s="2">
+        <v>60</v>
+      </c>
+      <c r="I25" s="2">
         <v>66</v>
-      </c>
-      <c r="I25" s="2">
-        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1216,28 +1231,173 @@
         <v>33</v>
       </c>
       <c r="B26" s="2">
-        <v>869.643886</v>
+        <v>870.8744369999999</v>
       </c>
       <c r="C26" s="2">
-        <v>262.298498</v>
+        <v>238.912853</v>
       </c>
       <c r="D26" s="2">
-        <v>-0.933485</v>
+        <v>0.355134</v>
       </c>
       <c r="E26" s="2">
-        <v>2.552094</v>
+        <v>13.098271</v>
       </c>
       <c r="F26" s="2">
+        <v>50</v>
+      </c>
+      <c r="G26" s="2">
+        <v>3</v>
+      </c>
+      <c r="H26" s="2">
+        <v>64</v>
+      </c>
+      <c r="I26" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="2">
+        <v>867.404531</v>
+      </c>
+      <c r="C27" s="2">
+        <v>295.248265</v>
+      </c>
+      <c r="D27" s="2">
+        <v>-0.919385</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5.539313</v>
+      </c>
+      <c r="F27" s="2">
+        <v>46.875</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>60</v>
+      </c>
+      <c r="I27" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="2">
+        <v>882.305206</v>
+      </c>
+      <c r="C28" s="2">
+        <v>218.405823</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.339119</v>
+      </c>
+      <c r="E28" s="2">
+        <v>9.654825000000001</v>
+      </c>
+      <c r="F28" s="2">
+        <v>54.6875</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3</v>
+      </c>
+      <c r="H28" s="2">
+        <v>70</v>
+      </c>
+      <c r="I28" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="2">
+        <v>871.8049549999999</v>
+      </c>
+      <c r="C29" s="2">
+        <v>239.230092</v>
+      </c>
+      <c r="D29" s="2">
+        <v>-0.289547</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2.65072</v>
+      </c>
+      <c r="F29" s="2">
         <v>45.3125</v>
       </c>
-      <c r="G26" s="2">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
+      <c r="G29" s="2">
+        <v>2</v>
+      </c>
+      <c r="H29" s="2">
         <v>58</v>
       </c>
-      <c r="I26" s="2">
-        <v>70</v>
+      <c r="I29" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="2">
+        <v>859.4885839999999</v>
+      </c>
+      <c r="C30" s="2">
+        <v>233.068891</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1.035501</v>
+      </c>
+      <c r="E30" s="2">
+        <v>8.482517</v>
+      </c>
+      <c r="F30" s="2">
+        <v>50</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>64</v>
+      </c>
+      <c r="I30" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="2">
+        <v>867.540967</v>
+      </c>
+      <c r="C31" s="2">
+        <v>277.950326</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.349355</v>
+      </c>
+      <c r="E31" s="2">
+        <v>8.73907</v>
+      </c>
+      <c r="F31" s="2">
+        <v>48.4375</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <v>62</v>
+      </c>
+      <c r="I31" s="2">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>